<commit_message>
feat: cancelar reserva front
</commit_message>
<xml_diff>
--- a/atividade-4/ms/cruise_data.xlsx
+++ b/atividade-4/ms/cruise_data.xlsx
@@ -808,7 +808,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>2000</v>
+        <v>2004</v>
       </c>
       <c r="K7" t="n">
         <v>8700</v>
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>1100</v>
+        <v>1103</v>
       </c>
       <c r="K11" t="n">
         <v>38356</v>

</xml_diff>

<commit_message>
feat: tudo pronto acho
</commit_message>
<xml_diff>
--- a/atividade-4/ms/cruise_data.xlsx
+++ b/atividade-4/ms/cruise_data.xlsx
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>2200</v>
+        <v>2201</v>
       </c>
       <c r="K3" t="n">
         <v>7900</v>
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>1200</v>
+        <v>1203</v>
       </c>
       <c r="K4" t="n">
         <v>3800</v>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>3000</v>
+        <v>3002</v>
       </c>
       <c r="K8" t="n">
         <v>9200</v>
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>1103</v>
+        <v>1119</v>
       </c>
       <c r="K11" t="n">
         <v>38356</v>

</xml_diff>